<commit_message>
feat: test different algorithms
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -5,16 +5,20 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Onedrive\Polito\OneDrive - Politecnico di Torino\Universita\Anno 4\DataScienceLab\Assignment\github\trajectories_particles\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://politoit-my.sharepoint.com/personal/s327134_studenti_polito_it/Documents/Universita/Anno 4/DataScienceLab/Assignment/github/trajectories_particles/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26B0BC77-899A-4E74-9CCE-F4514414D13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="54" documentId="13_ncr:1_{26B0BC77-899A-4E74-9CCE-F4514414D13E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E1922531-5A4B-42F2-9139-4BD2B4C4DBE2}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RandomForest" sheetId="1" r:id="rId1"/>
-    <sheet name="Knn R" sheetId="2" r:id="rId2"/>
+    <sheet name="ExtraTreesRegressor" sheetId="3" r:id="rId2"/>
+    <sheet name="Voting regressors" sheetId="4" r:id="rId3"/>
+    <sheet name="SVR" sheetId="5" r:id="rId4"/>
+    <sheet name="Ada boost regressor" sheetId="6" r:id="rId5"/>
+    <sheet name="Knn R" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="29">
   <si>
     <t>Random test and train set</t>
   </si>
@@ -86,14 +90,42 @@
   </si>
   <si>
     <t>4.85</t>
+  </si>
+  <si>
+    <t>NO TRIANGLE</t>
+  </si>
+  <si>
+    <t>Between RandomForest and ExtraTreesRegressor</t>
+  </si>
+  <si>
+    <t>21.66</t>
+  </si>
+  <si>
+    <t>Train on more than one and do the avg of the results</t>
+  </si>
+  <si>
+    <t>Step 10000</t>
+  </si>
+  <si>
+    <t>Time for the computations:</t>
+  </si>
+  <si>
+    <t>15.64</t>
+  </si>
+  <si>
+    <t>If I counted right 36 regressors were created</t>
+  </si>
+  <si>
+    <t>The single results are present on the notebook(more or 18 is the distance of each)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.000"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="#,##0.000"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
@@ -137,21 +169,29 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="46" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,8 +474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J31" sqref="J31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -455,26 +495,26 @@
       </c>
     </row>
     <row r="4" spans="1:20" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="1" t="s">
+      <c r="A4" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
-      <c r="H4" s="1"/>
-      <c r="M4" s="1" t="s">
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="M4" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
-      <c r="Q4" s="1"/>
-      <c r="R4" s="1"/>
-      <c r="S4" s="1"/>
-      <c r="T4" s="1"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -630,7 +670,7 @@
       <c r="A24" t="s">
         <v>7</v>
       </c>
-      <c r="B24" s="5">
+      <c r="B24" s="4">
         <v>4774</v>
       </c>
       <c r="C24">
@@ -639,10 +679,10 @@
       <c r="M24" t="s">
         <v>7</v>
       </c>
-      <c r="N24" s="4">
+      <c r="N24" s="3">
         <v>4.8949999999999996</v>
       </c>
-      <c r="O24" s="3">
+      <c r="O24" s="2">
         <v>0.31805555555555554</v>
       </c>
     </row>
@@ -650,7 +690,7 @@
       <c r="A25" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B25" s="4">
         <v>4755</v>
       </c>
       <c r="C25">
@@ -659,16 +699,16 @@
       <c r="M25" t="s">
         <v>8</v>
       </c>
-      <c r="N25" s="2" t="s">
+      <c r="N25" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="O25" s="3"/>
+      <c r="O25" s="2"/>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B26" s="4">
         <v>4801</v>
       </c>
       <c r="C26">
@@ -677,7 +717,7 @@
       <c r="M26" t="s">
         <v>9</v>
       </c>
-      <c r="O26" s="3"/>
+      <c r="O26" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -689,6 +729,276 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F003F4E8-D593-4BFF-87E3-29D5C075368A}">
+  <dimension ref="A3:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="5">
+        <v>4.7610000000000001</v>
+      </c>
+      <c r="C6" s="2">
+        <v>8.4027777777777771E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="5">
+        <v>4.7939999999999996</v>
+      </c>
+      <c r="C7" s="2">
+        <v>9.3055555555555558E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="5">
+        <v>4.8289999999999997</v>
+      </c>
+      <c r="C8" s="2">
+        <v>8.819444444444445E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C81B0295-B41E-4F3C-A2CD-675B272EA5B2}">
+  <dimension ref="A2:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="4">
+        <v>4703</v>
+      </c>
+      <c r="C6" s="6">
+        <v>1.0361111111111112</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="2"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C152FD2E-1142-4598-8207-69233640409F}">
+  <dimension ref="A4:G7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="30.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="G5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="9">
+        <v>0.10076388888888889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75105349-431A-4890-9659-36FF40B35EF2}">
+  <dimension ref="A3:G6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I9" sqref="I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.39374999999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4115DE50-951A-47A2-A7C2-60D96323A5AC}">
   <dimension ref="A2:H5"/>
   <sheetViews>

</xml_diff>